<commit_message>
???????????? ???????? ?????? ????????????? ??????
</commit_message>
<xml_diff>
--- a/src/tests/test_data/linux/xlsx/test_merge.xlsx
+++ b/src/tests/test_data/linux/xlsx/test_merge.xlsx
@@ -44,7 +44,7 @@
             <family val="2"/>
             <sz val="10"/>
           </rPr>
-          <t xml:space="preserve">+s2-s2</t>
+          <t xml:space="preserve">+s2</t>
         </r>
       </text>
     </comment>
@@ -57,7 +57,59 @@
             <family val="2"/>
             <sz val="10"/>
           </rPr>
+          <t xml:space="preserve">-s2</t>
+        </r>
+      </text>
+    </comment>
+    <comment authorId="0" ref="D1">
+      <text>
+        <r>
+          <rPr>
+            <rFont val="Arial"/>
+            <charset val="1"/>
+            <family val="2"/>
+            <sz val="10"/>
+          </rPr>
           <t xml:space="preserve">+s3-s3</t>
+        </r>
+      </text>
+    </comment>
+    <comment authorId="0" ref="E1">
+      <text>
+        <r>
+          <rPr>
+            <rFont val="Arial"/>
+            <charset val="1"/>
+            <family val="2"/>
+            <sz val="10"/>
+          </rPr>
+          <t xml:space="preserve">+s4-s4</t>
+        </r>
+      </text>
+    </comment>
+    <comment authorId="0" ref="F3">
+      <text>
+        <r>
+          <rPr>
+            <rFont val="Arial"/>
+            <charset val="1"/>
+            <family val="2"/>
+            <sz val="10"/>
+          </rPr>
+          <t xml:space="preserve">+s5</t>
+        </r>
+      </text>
+    </comment>
+    <comment authorId="0" ref="H5">
+      <text>
+        <r>
+          <rPr>
+            <rFont val="Arial"/>
+            <charset val="1"/>
+            <family val="2"/>
+            <sz val="10"/>
+          </rPr>
+          <t xml:space="preserve">-s5</t>
         </r>
       </text>
     </comment>
@@ -66,15 +118,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>#p1#</t>
   </si>
   <si>
-    <t>#p2#</t>
+    <t>#p21#</t>
+  </si>
+  <si>
+    <t>#p22#</t>
   </si>
   <si>
     <t>#p3#</t>
+  </si>
+  <si>
+    <t>#p4#</t>
+  </si>
+  <si>
+    <t>#p5#</t>
   </si>
 </sst>
 </file>
@@ -122,8 +183,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FF420E"/>
-        <bgColor rgb="00FF0000"/>
+        <fgColor rgb="00FF0000"/>
+        <bgColor rgb="00993300"/>
       </patternFill>
     </fill>
   </fills>
@@ -168,7 +229,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
@@ -176,6 +237,7 @@
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
     </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="0" numFmtId="164" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -185,66 +247,6 @@
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF420E"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -253,14 +255,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F15" activeCellId="0" pane="topLeft" sqref="F15"/>
+      <selection activeCell="H5" activeCellId="0" pane="topLeft" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9294117647059"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
@@ -270,8 +272,19 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
+      <c r="F3" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -298,7 +311,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9294117647059"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -323,7 +336,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9294117647059"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>